<commit_message>
try different templates and small fix
</commit_message>
<xml_diff>
--- a/results/results_parameter_testing.xlsx
+++ b/results/results_parameter_testing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="404">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1381,6 +1381,230 @@
   </si>
   <si>
     <t xml:space="preserve"> 52.18755264185059
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mask_01.vtk
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.3926833677141874
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.0314726918915678
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.26489787688798044
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7600476611763216
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.0277075828332634
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.772498106962496
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5.33055470049103
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20.272240183799003
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 71.62598275812971
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 94.10247184069144
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 69.1025917819341
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 68.15191786583149
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 64.65104088607714
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mask_02.vtk
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.4373899324715347
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.1170845689556579
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.32112101507938834
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.6902016619337479
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.1030417905326813
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.6429802035152223
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6.431407656020065
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 72.64165987741085
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19.79589315624266
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 93.30029699701637
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 56.11929817798953
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 62.38243897133723
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 60.84791743599933
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mask_04.vtk
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.43388334231223
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.0149048194790486
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.3236543978383953
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7662460558113806
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.144842288192387
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.6667852167232455
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6.0562791602653085
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 65.2162525193901
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 60.094306984538576
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95.30408078022428
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16.22260601495686
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 65.94857783792861
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 60.557164827407675
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mask_05.vtk
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.5294790284563924
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.0835121051448278
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.2601479275466791
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.8182787769669063
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.1391222991510368
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.9703321066752162
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7.040165472553342
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 62.81028922143926
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 53.00087159658319
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 85.34230186030939
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 59.64942912310182
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18.23559810113121
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 55.80769798051297
 </t>
   </si>
 </sst>
@@ -1713,18 +1937,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB27"/>
+  <dimension ref="A1:AG27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:33">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1809,8 +2033,23 @@
       <c r="AB2" t="s">
         <v>24</v>
       </c>
+      <c r="AC2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:33">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1895,8 +2134,23 @@
       <c r="AB3" t="s">
         <v>308</v>
       </c>
+      <c r="AC3" t="s">
+        <v>308</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>308</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>308</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>308</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>308</v>
+      </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:33">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1981,8 +2235,23 @@
       <c r="AB4" t="s">
         <v>26</v>
       </c>
+      <c r="AC4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:33">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2067,8 +2336,23 @@
       <c r="AB5" t="s">
         <v>26</v>
       </c>
+      <c r="AC5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2153,8 +2437,23 @@
       <c r="AB6" t="s">
         <v>224</v>
       </c>
+      <c r="AC6" t="s">
+        <v>238</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>238</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>238</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>238</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>238</v>
+      </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2239,8 +2538,23 @@
       <c r="AB7" t="s">
         <v>29</v>
       </c>
+      <c r="AC7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:33">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2325,8 +2639,23 @@
       <c r="AB8" t="s">
         <v>30</v>
       </c>
+      <c r="AC8" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>362</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>376</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>390</v>
+      </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:33">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2411,8 +2740,23 @@
       <c r="AB9" t="s">
         <v>24</v>
       </c>
+      <c r="AC9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2497,8 +2841,23 @@
       <c r="AB10" t="s">
         <v>31</v>
       </c>
+      <c r="AC10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2583,8 +2942,23 @@
       <c r="AB11" t="s">
         <v>32</v>
       </c>
+      <c r="AC11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:33">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2669,8 +3043,23 @@
       <c r="AB12" t="s">
         <v>335</v>
       </c>
+      <c r="AC12" t="s">
+        <v>349</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>363</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>309</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>377</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>391</v>
+      </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:33">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2755,8 +3144,23 @@
       <c r="AB13" t="s">
         <v>336</v>
       </c>
+      <c r="AC13" t="s">
+        <v>350</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>364</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>310</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>378</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>392</v>
+      </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:33">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2841,8 +3245,23 @@
       <c r="AB14" t="s">
         <v>337</v>
       </c>
+      <c r="AC14" t="s">
+        <v>351</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>365</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>311</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>379</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>393</v>
+      </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:33">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2927,8 +3346,23 @@
       <c r="AB15" t="s">
         <v>338</v>
       </c>
+      <c r="AC15" t="s">
+        <v>352</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>366</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>312</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>380</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>394</v>
+      </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:33">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3013,8 +3447,23 @@
       <c r="AB16" t="s">
         <v>339</v>
       </c>
+      <c r="AC16" t="s">
+        <v>353</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>367</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>313</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>381</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>395</v>
+      </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:33">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -3099,8 +3548,23 @@
       <c r="AB17" t="s">
         <v>340</v>
       </c>
+      <c r="AC17" t="s">
+        <v>354</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>368</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>314</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>382</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>396</v>
+      </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:33">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3185,8 +3649,23 @@
       <c r="AB18" t="s">
         <v>341</v>
       </c>
+      <c r="AC18" t="s">
+        <v>355</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>369</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>315</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>383</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>397</v>
+      </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:33">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -3271,8 +3750,23 @@
       <c r="AB19" t="s">
         <v>24</v>
       </c>
+      <c r="AC19" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:33">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3357,8 +3851,23 @@
       <c r="AB20" t="s">
         <v>31</v>
       </c>
+      <c r="AC20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:33">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3443,8 +3952,23 @@
       <c r="AB21" t="s">
         <v>342</v>
       </c>
+      <c r="AC21" t="s">
+        <v>356</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>370</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>316</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>384</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>398</v>
+      </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:33">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3529,8 +4053,23 @@
       <c r="AB22" t="s">
         <v>343</v>
       </c>
+      <c r="AC22" t="s">
+        <v>357</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>371</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>317</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>385</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>399</v>
+      </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:33">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -3615,8 +4154,23 @@
       <c r="AB23" t="s">
         <v>344</v>
       </c>
+      <c r="AC23" t="s">
+        <v>358</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>372</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>318</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>386</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>400</v>
+      </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:33">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -3701,8 +4255,23 @@
       <c r="AB24" t="s">
         <v>345</v>
       </c>
+      <c r="AC24" t="s">
+        <v>359</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>373</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>319</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>387</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>401</v>
+      </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:33">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3787,8 +4356,23 @@
       <c r="AB25" t="s">
         <v>346</v>
       </c>
+      <c r="AC25" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>374</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>320</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>388</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>402</v>
+      </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:33">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -3873,8 +4457,23 @@
       <c r="AB26" t="s">
         <v>347</v>
       </c>
+      <c r="AC26" t="s">
+        <v>361</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>375</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>389</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>403</v>
+      </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:33">
       <c r="B27" t="s">
         <v>24</v>
       </c>
@@ -3954,6 +4553,21 @@
         <v>24</v>
       </c>
       <c r="AB27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG27" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>